<commit_message>
629 commit for javaee over
</commit_message>
<xml_diff>
--- a/doc/log/侯旭东.xlsx
+++ b/doc/log/侯旭东.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
   <si>
     <t xml:space="preserve">                     时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -33,84 +33,368 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2019.4.1/18:00~20:00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>本地库和远程库的交互方式、本地库初始化、签名设置、添加提交以及查看</t>
-  </si>
-  <si>
-    <t>2019.4.2/15:30~17:30</t>
-  </si>
-  <si>
-    <t>Git基本操作</t>
-  </si>
-  <si>
-    <t>2019.4.3/18:00~20:00</t>
-  </si>
-  <si>
-    <t>git链接github</t>
-  </si>
-  <si>
-    <t>2019.4.6/16:30~18：30</t>
-  </si>
-  <si>
-    <t>简单测试JDBC</t>
-  </si>
-  <si>
-    <t>2019.4.7/16:30~18：30</t>
-  </si>
-  <si>
-    <t>初步了解JDBC</t>
-  </si>
-  <si>
-    <t>2019.4.10/20:30~22：30</t>
-  </si>
-  <si>
-    <t>JDBC开发步骤</t>
-  </si>
-  <si>
-    <t>2019.4.11/20:30~22：30</t>
-  </si>
-  <si>
-    <t>JDBC连接MYSQL</t>
-  </si>
-  <si>
-    <t>2019.4.13/10:00~12：00</t>
-  </si>
-  <si>
-    <t>Statement、PreparedStatement基本用法</t>
-  </si>
-  <si>
-    <t>2019/4/15/20:00~22:00</t>
-  </si>
-  <si>
-    <t>ResultSet、Batch、ACID基本用法</t>
-  </si>
-  <si>
-    <t>2019/5/16/20:00~22:00</t>
-  </si>
-  <si>
-    <t>Maven基础</t>
-  </si>
-  <si>
-    <t>2019/5/17/20:00~22:00</t>
-  </si>
-  <si>
-    <t>JS基础</t>
-  </si>
-  <si>
-    <t>2019/5/22/15:00~18:00</t>
-  </si>
-  <si>
-    <t>完成协同开发，并再次完善自己的实体类和测试类</t>
+    <t>2019/5/13 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019/6/19 20:30-21.30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019.4.1/18:00-20:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019.4.2/15:30-17:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019.4.3/18:00-20:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019.4.6/16:30-18:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019.4.7/16:30-18:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019.4.10/20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019.4.11/20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019.4.13/10:00-12:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/5/15 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/5/17 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/5/19 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/5/22 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/5/24 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/5/26 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/5/30 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/6/1 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/6/2 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/6/3 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/6/5 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/6/6 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/6/18 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/6/17 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/6/16 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/6/14 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/6/13 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/6/11 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/6/10 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/6/9 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/6/7 20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>web层基础配置</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>配置spring的应用上下文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>web层的搭建，基础整合spring-MVC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目运行出现错误，重构项目</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学习jquery-ajax</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>对测试的调试，处理遇到的问题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">   web层controller</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完善service层测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> web层的controller的书写</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>小组讨论，完善web层</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完善项目计划</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 测试web层是否返回json数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实现json展示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>写web层dish的js</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>初步了解Vue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Vue.js模板起步</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接口测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>调用接口实现增加删除修改功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 完善接口</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>client更新编辑功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 测试功能的实现</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>添加测试数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                         Git基本操作</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                        git链接github</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                       简单测试JDBC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                        初步了解JDBC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                        JDBC开发步骤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                      JDBC连接MYSQL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                                 Statement、PreparedStatement基本用法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                                        ResultSet、Batch、ACID基本用法</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019/5/14 20:30-22:30</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">          本地库和远程库的交互方式、本地库初始化、签名设置、添加提交以及查看</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>写road的测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>road模块一对多关系</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019.4.14/20:30-22:30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                                        学习mybatis映射文件多参数处理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019/4/15 20:00-22:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019/04/16/18:00 -22:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                    学习spring-data-jpa  </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019/04/18/15:00 - 18:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                        配置日志输出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019/4/20 20:00-22:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019/4/21 20:00-22:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                        了解http协议</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                          引入mybatis-3和mybatis-spring的依赖包</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019/4/22 20:00-22:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019/4/25 20:00-22:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">                                </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="等线"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                   学习maven常用命令</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                                            配置IDE的spring应用上下文</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019/4/29 20:00-22:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                   学习SpringMVC原理</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019/5/2 20:00-22:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                              编写dao层实体类road与接口roadDao</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019/5/5 20:00-22:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">                                          编写dao层实体测试roadTest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +407,33 @@
       <sz val="9"/>
       <name val="等线"/>
       <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -149,8 +460,23 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -459,7 +785,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -467,10 +793,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -493,18 +819,18 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -512,83 +838,332 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>18</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>19</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>21</v>
+        <v>70</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
-        <v>23</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.5" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>79</v>
+      </c>
+      <c r="C16" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>85</v>
+      </c>
+      <c r="C19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B35" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B37" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B40" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B41" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B42" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B43" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
-        <v>26</v>
+      <c r="C43" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>4</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
702 commit for doc
</commit_message>
<xml_diff>
--- a/doc/log/侯旭东.xlsx
+++ b/doc/log/侯旭东.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420"/>
+    <workbookView xWindow="0" yWindow="2540" windowWidth="14570" windowHeight="3920"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
   <si>
     <t xml:space="preserve">                     时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -34,10 +35,6 @@
   </si>
   <si>
     <t>2019/5/13 20:30-22:30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">       2019/6/19 20:30-21.30</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -387,6 +384,18 @@
   </si>
   <si>
     <t xml:space="preserve">                                          编写dao层实体测试roadTest</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019/6/19 20:30-21.30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">       2019/6/20 20:30-21.30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 写度量报告</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -785,7 +794,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -793,10 +802,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -819,154 +828,154 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>70</v>
+      </c>
+      <c r="C12" t="s">
         <v>71</v>
-      </c>
-      <c r="C12" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
         <v>73</v>
-      </c>
-      <c r="C13" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.5" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" t="s">
         <v>80</v>
-      </c>
-      <c r="C17" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" t="s">
         <v>83</v>
-      </c>
-      <c r="C18" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C19" t="s">
         <v>85</v>
-      </c>
-      <c r="C19" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" t="s">
         <v>87</v>
-      </c>
-      <c r="C20" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="15" x14ac:dyDescent="0.3">
@@ -974,191 +983,199 @@
         <v>3</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B25" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B34" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B35" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B39" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B40" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="43" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="15" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>4</v>
+        <v>88</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" ht="15" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>